<commit_message>
added lazy saving feature to more attributes and added spare saving for dates
</commit_message>
<xml_diff>
--- a/Datenstruktur.xlsx
+++ b/Datenstruktur.xlsx
@@ -21,6 +21,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Datums können immer weggelassen werden wenn nicht gesetzt!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -884,23 +892,39 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1100"/>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>- text</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1100"/>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>-</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="de-DE" sz="1100"/>
-            <a:t>lastModified</a:t>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>lastModified (das wird sowieso immer geändert!)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1287,17 +1311,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J23" sqref="I23:J23"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adjusted panels while resizing window for detailed todo editor
</commit_message>
<xml_diff>
--- a/Datenstruktur.xlsx
+++ b/Datenstruktur.xlsx
@@ -457,7 +457,7 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="lt1"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
@@ -469,7 +469,7 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
@@ -479,6 +479,9 @@
             <a:t> planStart, planEnd</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
             <a:effectLst/>
           </a:endParaRPr>
         </a:p>
@@ -493,9 +496,24 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>- reminderIsActive, reminderDate</a:t>
+            <a:t>- reminderIsActive, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>reminderDate</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
             <a:effectLst/>
           </a:endParaRPr>
         </a:p>
@@ -1314,7 +1332,7 @@
   <dimension ref="E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>